<commit_message>
probar en placa volumen logaritmico
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Vivado-Workspace\DSED_LAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\DSED_LAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B153723-3BBF-410D-A8F7-D4CFBBB55D93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8191F67-D7DD-4F4E-A52E-8DE5955BC23F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{E5AB915A-C1D5-4433-96F4-39BD5765E129}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{E5AB915A-C1D5-4433-96F4-39BD5765E129}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,6 +31,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>NIVEL</t>
+  </si>
+  <si>
+    <t>FACTOR NUM</t>
+  </si>
+  <si>
+    <t>FACTOR DEN</t>
+  </si>
+  <si>
+    <t>FACTOR</t>
+  </si>
+  <si>
+    <t>VOLUMEN (vol)</t>
+  </si>
+  <si>
+    <t>sample_in=</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -84,7 +108,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -386,12 +410,12 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -420,7 +444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -445,11 +469,11 @@
         <v>1</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G21" si="2">DEC2BIN(F2)</f>
+        <f t="shared" ref="G2:G20" si="2">DEC2BIN(F2)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -466,7 +490,7 @@
         <v>7.9295526932425323E-2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E2:E21" si="3">D3*2^5</f>
+        <f t="shared" ref="E3:E21" si="3">D3*2^5</f>
         <v>2.5374568618376103</v>
       </c>
       <c r="F3">
@@ -478,7 +502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -507,7 +531,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -536,7 +560,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -565,7 +589,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -594,7 +618,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -623,7 +647,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -652,7 +676,7 @@
         <v>10011</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -681,7 +705,7 @@
         <v>11001</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -710,7 +734,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -739,7 +763,7 @@
         <v>101000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -768,7 +792,7 @@
         <v>110001</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -797,7 +821,7 @@
         <v>111101</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -826,7 +850,7 @@
         <v>1001011</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -855,7 +879,7 @@
         <v>1011101</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -884,7 +908,7 @@
         <v>1110010</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -913,7 +937,7 @@
         <v>10001100</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -942,7 +966,7 @@
         <v>10101011</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -971,7 +995,7 @@
         <v>11010001</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1004,4 +1028,747 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D65327-0BF3-452A-8D8D-CFB3EDFEBD7E}">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>7^(A2/10)-1</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <f>B2/C2</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>D2*2^5</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>TRUNC(E2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" t="str">
+        <f>DEC2BIN(F2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>(B24/8)*D2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B22" si="0">7^(A3/10)-1</f>
+        <v>0.2148140440390669</v>
+      </c>
+      <c r="C3">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D22" si="1">B3/C3</f>
+        <v>3.5802340673177814E-2</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E22" si="2">D3*2^5</f>
+        <v>1.14567490154169</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F22" si="3">TRUNC(E3)</f>
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G22" si="4">DEC2BIN(F3)</f>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f>(B24/8)*D3</f>
+        <v>1.1411996089575429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0.47577316159455196</v>
+      </c>
+      <c r="C4">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>7.9295526932425323E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>2.5374568618376103</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <f>(B24/8)*D4</f>
+        <v>2.527544920971057</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>0.79278996252099709</v>
+      </c>
+      <c r="C5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>0.13213166042016619</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>4.2282131334453181</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <f>(B24/8)*D5</f>
+        <v>4.2116966758927976</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>1.1779064244827797</v>
+      </c>
+      <c r="C6">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>0.19631773741379663</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>6.2821675972414921</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="4"/>
+        <v>110</v>
+      </c>
+      <c r="H6">
+        <f>(B24/8)*D6</f>
+        <v>6.2576278800647671</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>1.6457513110645907</v>
+      </c>
+      <c r="C7">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0.2742918851774318</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>8.7773403256778177</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="H7">
+        <f>(B24/8)*D7</f>
+        <v>8.7430538400306386</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>2.2140958497160383</v>
+      </c>
+      <c r="C8">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0.36901597495267308</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>11.808511198485538</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="4"/>
+        <v>1011</v>
+      </c>
+      <c r="H8">
+        <f>(B24/8)*D8</f>
+        <v>11.762384201616454</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>2.9045287771227213</v>
+      </c>
+      <c r="C9">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0.48408812952045355</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>15.490820144654514</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="4"/>
+        <v>1111</v>
+      </c>
+      <c r="H9">
+        <f>(B24/8)*D9</f>
+        <v>15.430309128464456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>3.7432763938033666</v>
+      </c>
+      <c r="C10">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>0.62387939896722777</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>19.964140766951289</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="4"/>
+        <v>10011</v>
+      </c>
+      <c r="H10">
+        <f>(B24/8)*D10</f>
+        <v>19.886155842080385</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>4.7621987779513102</v>
+      </c>
+      <c r="C11">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>0.79369979632521837</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>25.398393482406988</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="4"/>
+        <v>11001</v>
+      </c>
+      <c r="H11">
+        <f>(B24/8)*D11</f>
+        <v>25.299181007866334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="4"/>
+        <v>100000</v>
+      </c>
+      <c r="H12">
+        <f>(B24/8)*D12</f>
+        <v>31.875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>7.5036983082734707</v>
+      </c>
+      <c r="C13">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>1.2506163847122451</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>40.019724310791844</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="4"/>
+        <v>101000</v>
+      </c>
+      <c r="H13">
+        <f>(B24/8)*D13</f>
+        <v>39.863397262702811</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>9.3304121311618644</v>
+      </c>
+      <c r="C14">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>1.5550686885269773</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>49.762198032863274</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="4"/>
+        <v>110001</v>
+      </c>
+      <c r="H14">
+        <f>(B24/8)*D14</f>
+        <v>49.567814446797399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>11.549529737646981</v>
+      </c>
+      <c r="C15">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>1.9249216229411636</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>61.597491934117237</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="4"/>
+        <v>111101</v>
+      </c>
+      <c r="H15">
+        <f>(B24/8)*D15</f>
+        <v>61.356876731249592</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>14.245344971379454</v>
+      </c>
+      <c r="C16">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>2.3742241618965756</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>75.975173180690419</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="4"/>
+        <v>1001011</v>
+      </c>
+      <c r="H16">
+        <f>(B24/8)*D16</f>
+        <v>75.678395160453348</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>17.520259177452129</v>
+      </c>
+      <c r="C17">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>2.9200431962420215</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>93.441382279744687</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="4"/>
+        <v>1011101</v>
+      </c>
+      <c r="H17">
+        <f>(B24/8)*D17</f>
+        <v>93.07637688021444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>21.498670948012268</v>
+      </c>
+      <c r="C18">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>3.5831118246687113</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>114.65957838939876</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="4"/>
+        <v>1110010</v>
+      </c>
+      <c r="H18">
+        <f>(B24/8)*D18</f>
+        <v>114.21168941131518</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>26.331701439859053</v>
+      </c>
+      <c r="C19">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>4.3886169066431755</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>140.43574101258162</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="4"/>
+        <v>10001100</v>
+      </c>
+      <c r="H19">
+        <f>(B24/8)*D19</f>
+        <v>139.88716389925122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>32.20293475662357</v>
+      </c>
+      <c r="C20">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>5.3671557927705953</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>171.74898536865905</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>171</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="4"/>
+        <v>10101011</v>
+      </c>
+      <c r="H20">
+        <f>(B24/8)*D20</f>
+        <v>171.07809089456273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>39.335391445659155</v>
+      </c>
+      <c r="C21">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>6.5558985742765259</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>209.78875437684883</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>209</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="4"/>
+        <v>11010001</v>
+      </c>
+      <c r="H21">
+        <f>(B24/8)*D21</f>
+        <v>208.96926705506425</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C22">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>256</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>256</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="4"/>
+        <v>100000000</v>
+      </c>
+      <c r="H22">
+        <f>(B24/8)*D22</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>